<commit_message>
Corrected "Trim activé" en "Trim désactivé"
</commit_message>
<xml_diff>
--- a/OptimisationPCWindows/OptimisationPCWindows.xlsx
+++ b/OptimisationPCWindows/OptimisationPCWindows.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\perso\autres\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\programation\notices\OptimisationPCWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9724A3E3-97B3-418D-9CE6-E69BB7E3D434}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="171" xr2:uid="{BE25C07D-5904-4AEC-8632-5F7E6FCC6B94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="171" xr2:uid="{BE25C07D-5904-4AEC-8632-5F7E6FCC6B94}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -50,9 +51,6 @@
     <t>Force le système à vérifier que chaque suppression sur le SSD est bien faite, pour que la réécriture soit plus rapide, au lieu de devoir effacer une cellule avant de réécrire dedans quand on en a besoin.</t>
   </si>
   <si>
-    <t>ouvrir le cmd. Taper "fsutil behavior query DisableDeleteNotify". Si on retourne 0 : Trim activé, c'est bon ! Sinon, taper "fsutil behavior set DisableDeleteNotify 0" pour l'activer.</t>
-  </si>
-  <si>
     <t>ouvrir le cmd. Taper "fsutil behavior set disablelastaccess 1"</t>
   </si>
   <si>
@@ -201,6 +199,9 @@
   </si>
   <si>
     <t>Panneau de configuration --&gt; Programmes --&gt; Programmes et fonctionnalités. Cliquez sur les logiciels que vous n'utilisez plus, et cliquez sur "désinstaller"</t>
+  </si>
+  <si>
+    <t>ouvrir le cmd. Taper "fsutil behavior query DisableDeleteNotify". Si on retourne 0 : Trim déactivé, c'est bon ! Sinon, taper "fsutil behavior set DisableDeleteNotify 0" pour le désactiver.</t>
   </si>
 </sst>
 </file>
@@ -542,9 +543,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,62 +560,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,343 +939,343 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="58" style="3" customWidth="1"/>
-    <col min="3" max="3" width="95.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="100.85546875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="58" style="2" customWidth="1"/>
+    <col min="3" max="3" width="95.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="100.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="7" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="7" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B17" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="1:4" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
+      <c r="B22" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" s="8" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" s="8" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>